<commit_message>
ML project + gitignore for R + skull-stripping
- Datasets created for ML
- Risk factors evaluation EDA
- Skull-stripping algorithm improved
</commit_message>
<xml_diff>
--- a/Demo/evaluation/eval_results.xlsx
+++ b/Demo/evaluation/eval_results.xlsx
@@ -428,16 +428,16 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.9792160143620312</v>
+        <v>0.2109475628992479</v>
       </c>
       <c r="C1" t="n">
-        <v>0.2520240180571169</v>
+        <v>0.08490505198392986</v>
       </c>
       <c r="D1" t="n">
-        <v>0.02078398563796875</v>
+        <v>0.7890524371007521</v>
       </c>
       <c r="E1" t="n">
-        <v>0.7821064134868375</v>
+        <v>0.1944387322314474</v>
       </c>
     </row>
     <row r="2">
@@ -447,16 +447,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9634843206735871</v>
+        <v>0.1471589290444466</v>
       </c>
       <c r="C2" t="n">
-        <v>0.06368273833025961</v>
+        <v>0.03137031465275244</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03651567932641287</v>
+        <v>0.8528410709555534</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9058004665808893</v>
+        <v>0.1426829209196241</v>
       </c>
     </row>
     <row r="3">
@@ -466,16 +466,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9836128986144017</v>
+        <v>0.916350101644176</v>
       </c>
       <c r="C3" t="n">
-        <v>0.09169629098614822</v>
+        <v>0.04528999598468715</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01638710138559827</v>
+        <v>0.083649898355824</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9009949990082746</v>
+        <v>0.8766467728230319</v>
       </c>
     </row>
     <row r="4">
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9761554301617256</v>
+        <v>0.0002450104830821196</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03525813070093572</v>
+        <v>0.0007696321663228415</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02384456983827438</v>
+        <v>0.9997549895169179</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9429101798029891</v>
+        <v>0.0002448220601496031</v>
       </c>
     </row>
     <row r="5">
@@ -504,16 +504,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9868262931921268</v>
+        <v>0.1204399631601514</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4353437584721077</v>
+        <v>0.07714737285349238</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01317370680787327</v>
+        <v>0.8795600368398485</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6875191307778298</v>
+        <v>0.1118138206484147</v>
       </c>
     </row>
     <row r="6">
@@ -523,16 +523,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9883753170220559</v>
+        <v>0.9284232586389959</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1486449770260433</v>
+        <v>0.1248679750926145</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01162468297794407</v>
+        <v>0.07157674136100409</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8604706735244326</v>
+        <v>0.8253619795359144</v>
       </c>
     </row>
     <row r="7">
@@ -542,16 +542,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9134165510438322</v>
+        <v>0.8149335533624349</v>
       </c>
       <c r="C7" t="n">
-        <v>0.004165879202179395</v>
+        <v>0.09273143389216423</v>
       </c>
       <c r="D7" t="n">
-        <v>0.08658344895616781</v>
+        <v>0.1850664466375651</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9096271542004111</v>
+        <v>0.7457766181940515</v>
       </c>
     </row>
     <row r="8">
@@ -561,16 +561,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9103968844906973</v>
+        <v>0.8337670019782656</v>
       </c>
       <c r="C8" t="n">
-        <v>0.008046557714372519</v>
+        <v>0.08019858609828262</v>
       </c>
       <c r="D8" t="n">
-        <v>0.08960311550930268</v>
+        <v>0.1662329980217344</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9031297984439485</v>
+        <v>0.7718645559330557</v>
       </c>
     </row>
     <row r="9">
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5609534440843192</v>
+        <v>0.04089765958486836</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00429756122378742</v>
+        <v>0.02495737852755657</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4390465559156808</v>
+        <v>0.9591023404151316</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5585530282486886</v>
+        <v>0.03990181488680195</v>
       </c>
     </row>
     <row r="10">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9220974377613321</v>
+        <v>0.6919948240070778</v>
       </c>
       <c r="C10" t="n">
-        <v>0.007748717964380943</v>
+        <v>0.09746219560244221</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07790256223866784</v>
+        <v>0.3080051759929222</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9150073042255399</v>
+        <v>0.630540921391113</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2638054354417353</v>
+        <v>0.05337750321202273</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2047397035232575</v>
+        <v>0.003250118200348808</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7361945645582647</v>
+        <v>0.9466224967879773</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2189729737222382</v>
+        <v>0.0532045820316198</v>
       </c>
     </row>
     <row r="12">
@@ -637,16 +637,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.8978450335789924</v>
+        <v>0.1294709107830068</v>
       </c>
       <c r="C12" t="n">
-        <v>0.005166805007084706</v>
+        <v>0.02574808629088379</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1021549664210076</v>
+        <v>0.8705290892169932</v>
       </c>
       <c r="E12" t="n">
-        <v>0.893229888916461</v>
+        <v>0.1262209625476124</v>
       </c>
     </row>
     <row r="13">
@@ -656,16 +656,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9718471798524856</v>
+        <v>0.002815376490472596</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09345632812551666</v>
+        <v>0.007787633694954902</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02815282014751439</v>
+        <v>0.9971846235095274</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8887846316811734</v>
+        <v>0.002793620795038229</v>
       </c>
     </row>
     <row r="14">
@@ -675,16 +675,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9726691091744873</v>
+        <v>0.27242409839717</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03286424087874159</v>
+        <v>0.004044343969174593</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02733089082551269</v>
+        <v>0.72757590160283</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9417201900096364</v>
+        <v>0.2713267596530913</v>
       </c>
     </row>
     <row r="15">
@@ -694,16 +694,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9824920294664912</v>
+        <v>0.2981947965745748</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1565800879932391</v>
+        <v>0.1040242579877622</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01750797053350888</v>
+        <v>0.7018052034254252</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8494803253713239</v>
+        <v>0.2700980475900741</v>
       </c>
     </row>
     <row r="16">
@@ -713,16 +713,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9893086565790987</v>
+        <v>0.584195185130421</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1273801895937043</v>
+        <v>0.07555270781649608</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01069134342090131</v>
+        <v>0.415804814869579</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8775288635643269</v>
+        <v>0.5431581185048652</v>
       </c>
     </row>
     <row r="17">
@@ -732,16 +732,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9888894069049555</v>
+        <v>0.01198618216978764</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1520044347852188</v>
+        <v>0.01606460071924757</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01111059309504452</v>
+        <v>0.9880138178302124</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8584076389335474</v>
+        <v>0.01179667332303764</v>
       </c>
     </row>
     <row r="18">
@@ -751,16 +751,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9774012891113667</v>
+        <v>0.9274906325732896</v>
       </c>
       <c r="C18" t="n">
-        <v>0.05090809042361569</v>
+        <v>0.04490490510891151</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02259871088863327</v>
+        <v>0.07250936742671049</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9300540152063929</v>
+        <v>0.8876316189525555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conclusions and future lines added
</commit_message>
<xml_diff>
--- a/Demo/evaluation/eval_results.xlsx
+++ b/Demo/evaluation/eval_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,16 +428,16 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.4778617305899065</v>
+        <v>0.8621994474801085</v>
       </c>
       <c r="C1" t="n">
-        <v>0.3360785031416944</v>
+        <v>0.3218280216476248</v>
       </c>
       <c r="D1" t="n">
-        <v>0.5221382694100936</v>
+        <v>0.1378005525198916</v>
       </c>
       <c r="E1" t="n">
-        <v>0.3576599200318307</v>
+        <v>0.6522780825945866</v>
       </c>
     </row>
     <row r="2">
@@ -447,16 +447,320 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6076494921274338</v>
+        <v>0.8518972959555118</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4355800676052771</v>
+        <v>0.3646020234935835</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3923505078725662</v>
+        <v>0.1481027040444882</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4232780224798379</v>
+        <v>0.6242825976283755</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>IBSR_03</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.919355279505717</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1936610613459917</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08064472049428291</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.7701979307836657</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IBSR_04</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9624610274355632</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.2338914958918662</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.03753897256443682</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.7800207965124916</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>IBSR_05</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8785554010948127</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3811338059447518</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1214445989051874</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6361117201774994</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>IBSR_06</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9168950152773334</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.3741755108285925</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.08310498472266656</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.6672328301968279</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>IBSR_07</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.8915154350722085</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5419630222041938</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1084845649277914</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.5781691403972916</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>IBSR_08</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9506492370615794</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.6308630140296889</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.04935076293842058</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5829117644360738</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>IBSR_09</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8604519621838554</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.3538125892207827</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1395480378161446</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.6355768656864891</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>IBSR_10</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.7344269705475415</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.4308932660169187</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.2655730294524585</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.5132646773801071</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>IBSR_11</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.2664658565376535</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.09257409570209964</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.7335341434623466</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.2438881331580717</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>IBSR_12</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9757411692699818</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5913707020147395</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.02425883073001819</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.6131451132251298</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>IBSR_13</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.9726804557130886</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.2539923077867834</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.02731954428691143</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.7756670034362553</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>IBSR_14</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.9542135013741299</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.2335038645758613</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.04578649862587012</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.773579660978391</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>IBSR_15</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9178993337032967</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.2116059672908891</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.08210066629670333</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.7575889839463974</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>IBSR_16</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.9273415808237633</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.2180218071094901</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.07265841917623671</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.7613505566246426</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>IBSR_17</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9207039455154958</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.1650309777155875</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.07929605448450412</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.7902828020254258</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>IBSR_18</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.8757601387296264</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.1598735464828767</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1242398612703735</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.7550479458603252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>